<commit_message>
Updated for Week 6 deliverables
</commit_message>
<xml_diff>
--- a/Documents/Week6/06_Team3PMScheduleManagmentPlanGantt.xlsx
+++ b/Documents/Week6/06_Team3PMScheduleManagmentPlanGantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VisualStudioRepos\Documents\Week5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VisualStudioRepos\Documents\Week6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715714CA-FBE5-451F-A2ED-C9FA25FDF3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C74A6E-3B48-48E0-9B47-5D0955FA5AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -1570,9 +1570,6 @@
     <t>Week 7- Phase 3 Source</t>
   </si>
   <si>
-    <t>Phase 2 Source</t>
-  </si>
-  <si>
     <t>Phase 3 Source</t>
   </si>
   <si>
@@ -1613,6 +1610,9 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>Phase 2 Source (DB ISUD Access)</t>
   </si>
 </sst>
 </file>
@@ -2796,18 +2796,18 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3261,13 +3261,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>99060</xdr:colOff>
+          <xdr:colOff>95250</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>121920</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>106680</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:to>
@@ -3852,27 +3852,27 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="32" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.88671875" style="4" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" style="4" hidden="1" customWidth="1"/>
     <col min="5" max="6" width="12" style="1" customWidth="1"/>
     <col min="7" max="7" width="6" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="1.88671875" style="1" customWidth="1"/>
-    <col min="11" max="66" width="2.44140625" style="1" customWidth="1"/>
-    <col min="67" max="16384" width="9.109375" style="2"/>
+    <col min="8" max="8" width="6.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="1.85546875" style="1" customWidth="1"/>
+    <col min="11" max="66" width="2.42578125" style="1" customWidth="1"/>
+    <col min="67" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:143" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:143" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="67" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="41"/>
@@ -3880,33 +3880,33 @@
       <c r="E1" s="41"/>
       <c r="F1" s="41"/>
       <c r="I1" s="70"/>
-      <c r="K1" s="146" t="s">
+      <c r="K1" s="148" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="146"/>
-      <c r="M1" s="146"/>
-      <c r="N1" s="146"/>
-      <c r="O1" s="146"/>
-      <c r="P1" s="146"/>
-      <c r="Q1" s="146"/>
-      <c r="R1" s="146"/>
-      <c r="S1" s="146"/>
-      <c r="T1" s="146"/>
-      <c r="U1" s="146"/>
-      <c r="V1" s="146"/>
-      <c r="W1" s="146"/>
-      <c r="X1" s="146"/>
-      <c r="Y1" s="146"/>
-      <c r="Z1" s="146"/>
-      <c r="AA1" s="146"/>
-      <c r="AB1" s="146"/>
-      <c r="AC1" s="146"/>
-      <c r="AD1" s="146"/>
-      <c r="AE1" s="146"/>
-    </row>
-    <row r="2" spans="1:143" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L1" s="148"/>
+      <c r="M1" s="148"/>
+      <c r="N1" s="148"/>
+      <c r="O1" s="148"/>
+      <c r="P1" s="148"/>
+      <c r="Q1" s="148"/>
+      <c r="R1" s="148"/>
+      <c r="S1" s="148"/>
+      <c r="T1" s="148"/>
+      <c r="U1" s="148"/>
+      <c r="V1" s="148"/>
+      <c r="W1" s="148"/>
+      <c r="X1" s="148"/>
+      <c r="Y1" s="148"/>
+      <c r="Z1" s="148"/>
+      <c r="AA1" s="148"/>
+      <c r="AB1" s="148"/>
+      <c r="AC1" s="148"/>
+      <c r="AD1" s="148"/>
+      <c r="AE1" s="148"/>
+    </row>
+    <row r="2" spans="1:143" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="110" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B2" s="111"/>
       <c r="C2" s="111"/>
@@ -3974,7 +3974,7 @@
       <c r="BM2" s="114"/>
       <c r="BN2" s="114"/>
     </row>
-    <row r="3" spans="1:143" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:143" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="110"/>
       <c r="B3" s="66"/>
       <c r="C3" s="116"/>
@@ -4042,16 +4042,16 @@
       <c r="BM3" s="114"/>
       <c r="BN3" s="114"/>
     </row>
-    <row r="4" spans="1:143" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:143" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="118"/>
       <c r="B4" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="147">
+      <c r="C4" s="149">
         <v>44489</v>
       </c>
-      <c r="D4" s="147"/>
-      <c r="E4" s="147"/>
+      <c r="D4" s="149"/>
+      <c r="E4" s="149"/>
       <c r="F4" s="120"/>
       <c r="G4" s="119" t="s">
         <v>73</v>
@@ -4061,184 +4061,184 @@
       </c>
       <c r="I4" s="122"/>
       <c r="J4" s="123"/>
-      <c r="K4" s="148" t="str">
+      <c r="K4" s="146" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="148"/>
-      <c r="M4" s="148"/>
-      <c r="N4" s="148"/>
-      <c r="O4" s="148"/>
-      <c r="P4" s="148"/>
-      <c r="Q4" s="148"/>
-      <c r="R4" s="148" t="str">
+      <c r="L4" s="146"/>
+      <c r="M4" s="146"/>
+      <c r="N4" s="146"/>
+      <c r="O4" s="146"/>
+      <c r="P4" s="146"/>
+      <c r="Q4" s="146"/>
+      <c r="R4" s="146" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="148"/>
-      <c r="T4" s="148"/>
-      <c r="U4" s="148"/>
-      <c r="V4" s="148"/>
-      <c r="W4" s="148"/>
-      <c r="X4" s="148"/>
-      <c r="Y4" s="148" t="str">
+      <c r="S4" s="146"/>
+      <c r="T4" s="146"/>
+      <c r="U4" s="146"/>
+      <c r="V4" s="146"/>
+      <c r="W4" s="146"/>
+      <c r="X4" s="146"/>
+      <c r="Y4" s="146" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="148"/>
-      <c r="AA4" s="148"/>
-      <c r="AB4" s="148"/>
-      <c r="AC4" s="148"/>
-      <c r="AD4" s="148"/>
-      <c r="AE4" s="148"/>
-      <c r="AF4" s="148" t="str">
+      <c r="Z4" s="146"/>
+      <c r="AA4" s="146"/>
+      <c r="AB4" s="146"/>
+      <c r="AC4" s="146"/>
+      <c r="AD4" s="146"/>
+      <c r="AE4" s="146"/>
+      <c r="AF4" s="146" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="148"/>
-      <c r="AH4" s="148"/>
-      <c r="AI4" s="148"/>
-      <c r="AJ4" s="148"/>
-      <c r="AK4" s="148"/>
-      <c r="AL4" s="148"/>
-      <c r="AM4" s="148" t="str">
+      <c r="AG4" s="146"/>
+      <c r="AH4" s="146"/>
+      <c r="AI4" s="146"/>
+      <c r="AJ4" s="146"/>
+      <c r="AK4" s="146"/>
+      <c r="AL4" s="146"/>
+      <c r="AM4" s="146" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="148"/>
-      <c r="AO4" s="148"/>
-      <c r="AP4" s="148"/>
-      <c r="AQ4" s="148"/>
-      <c r="AR4" s="148"/>
-      <c r="AS4" s="148"/>
-      <c r="AT4" s="148" t="str">
+      <c r="AN4" s="146"/>
+      <c r="AO4" s="146"/>
+      <c r="AP4" s="146"/>
+      <c r="AQ4" s="146"/>
+      <c r="AR4" s="146"/>
+      <c r="AS4" s="146"/>
+      <c r="AT4" s="146" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="148"/>
-      <c r="AV4" s="148"/>
-      <c r="AW4" s="148"/>
-      <c r="AX4" s="148"/>
-      <c r="AY4" s="148"/>
-      <c r="AZ4" s="148"/>
-      <c r="BA4" s="148" t="str">
+      <c r="AU4" s="146"/>
+      <c r="AV4" s="146"/>
+      <c r="AW4" s="146"/>
+      <c r="AX4" s="146"/>
+      <c r="AY4" s="146"/>
+      <c r="AZ4" s="146"/>
+      <c r="BA4" s="146" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="148"/>
-      <c r="BC4" s="148"/>
-      <c r="BD4" s="148"/>
-      <c r="BE4" s="148"/>
-      <c r="BF4" s="148"/>
-      <c r="BG4" s="148"/>
-      <c r="BH4" s="148" t="str">
+      <c r="BB4" s="146"/>
+      <c r="BC4" s="146"/>
+      <c r="BD4" s="146"/>
+      <c r="BE4" s="146"/>
+      <c r="BF4" s="146"/>
+      <c r="BG4" s="146"/>
+      <c r="BH4" s="146" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="148"/>
-      <c r="BJ4" s="148"/>
-      <c r="BK4" s="148"/>
-      <c r="BL4" s="148"/>
-      <c r="BM4" s="148"/>
-      <c r="BN4" s="148"/>
-    </row>
-    <row r="5" spans="1:143" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI4" s="146"/>
+      <c r="BJ4" s="146"/>
+      <c r="BK4" s="146"/>
+      <c r="BL4" s="146"/>
+      <c r="BM4" s="146"/>
+      <c r="BN4" s="146"/>
+    </row>
+    <row r="5" spans="1:143" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="118"/>
       <c r="B5" s="119" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="147" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" s="147"/>
-      <c r="E5" s="147"/>
+      <c r="C5" s="149" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="149"/>
+      <c r="E5" s="149"/>
       <c r="F5" s="124"/>
       <c r="G5" s="124"/>
       <c r="H5" s="124"/>
       <c r="I5" s="124"/>
       <c r="J5" s="123"/>
-      <c r="K5" s="149">
+      <c r="K5" s="147">
         <f>K6</f>
         <v>44487</v>
       </c>
-      <c r="L5" s="149"/>
-      <c r="M5" s="149"/>
-      <c r="N5" s="149"/>
-      <c r="O5" s="149"/>
-      <c r="P5" s="149"/>
-      <c r="Q5" s="149"/>
-      <c r="R5" s="149">
+      <c r="L5" s="147"/>
+      <c r="M5" s="147"/>
+      <c r="N5" s="147"/>
+      <c r="O5" s="147"/>
+      <c r="P5" s="147"/>
+      <c r="Q5" s="147"/>
+      <c r="R5" s="147">
         <f>R6</f>
         <v>44494</v>
       </c>
-      <c r="S5" s="149"/>
-      <c r="T5" s="149"/>
-      <c r="U5" s="149"/>
-      <c r="V5" s="149"/>
-      <c r="W5" s="149"/>
-      <c r="X5" s="149"/>
-      <c r="Y5" s="149">
+      <c r="S5" s="147"/>
+      <c r="T5" s="147"/>
+      <c r="U5" s="147"/>
+      <c r="V5" s="147"/>
+      <c r="W5" s="147"/>
+      <c r="X5" s="147"/>
+      <c r="Y5" s="147">
         <f>Y6</f>
         <v>44501</v>
       </c>
-      <c r="Z5" s="149"/>
-      <c r="AA5" s="149"/>
-      <c r="AB5" s="149"/>
-      <c r="AC5" s="149"/>
-      <c r="AD5" s="149"/>
-      <c r="AE5" s="149"/>
-      <c r="AF5" s="149">
+      <c r="Z5" s="147"/>
+      <c r="AA5" s="147"/>
+      <c r="AB5" s="147"/>
+      <c r="AC5" s="147"/>
+      <c r="AD5" s="147"/>
+      <c r="AE5" s="147"/>
+      <c r="AF5" s="147">
         <f>AF6</f>
         <v>44508</v>
       </c>
-      <c r="AG5" s="149"/>
-      <c r="AH5" s="149"/>
-      <c r="AI5" s="149"/>
-      <c r="AJ5" s="149"/>
-      <c r="AK5" s="149"/>
-      <c r="AL5" s="149"/>
-      <c r="AM5" s="149">
+      <c r="AG5" s="147"/>
+      <c r="AH5" s="147"/>
+      <c r="AI5" s="147"/>
+      <c r="AJ5" s="147"/>
+      <c r="AK5" s="147"/>
+      <c r="AL5" s="147"/>
+      <c r="AM5" s="147">
         <f>AM6</f>
         <v>44515</v>
       </c>
-      <c r="AN5" s="149"/>
-      <c r="AO5" s="149"/>
-      <c r="AP5" s="149"/>
-      <c r="AQ5" s="149"/>
-      <c r="AR5" s="149"/>
-      <c r="AS5" s="149"/>
-      <c r="AT5" s="149">
+      <c r="AN5" s="147"/>
+      <c r="AO5" s="147"/>
+      <c r="AP5" s="147"/>
+      <c r="AQ5" s="147"/>
+      <c r="AR5" s="147"/>
+      <c r="AS5" s="147"/>
+      <c r="AT5" s="147">
         <f>AT6</f>
         <v>44522</v>
       </c>
-      <c r="AU5" s="149"/>
-      <c r="AV5" s="149"/>
-      <c r="AW5" s="149"/>
-      <c r="AX5" s="149"/>
-      <c r="AY5" s="149"/>
-      <c r="AZ5" s="149"/>
-      <c r="BA5" s="149">
+      <c r="AU5" s="147"/>
+      <c r="AV5" s="147"/>
+      <c r="AW5" s="147"/>
+      <c r="AX5" s="147"/>
+      <c r="AY5" s="147"/>
+      <c r="AZ5" s="147"/>
+      <c r="BA5" s="147">
         <f>BA6</f>
         <v>44529</v>
       </c>
-      <c r="BB5" s="149"/>
-      <c r="BC5" s="149"/>
-      <c r="BD5" s="149"/>
-      <c r="BE5" s="149"/>
-      <c r="BF5" s="149"/>
-      <c r="BG5" s="149"/>
-      <c r="BH5" s="149">
+      <c r="BB5" s="147"/>
+      <c r="BC5" s="147"/>
+      <c r="BD5" s="147"/>
+      <c r="BE5" s="147"/>
+      <c r="BF5" s="147"/>
+      <c r="BG5" s="147"/>
+      <c r="BH5" s="147">
         <f>BH6</f>
         <v>44536</v>
       </c>
-      <c r="BI5" s="149"/>
-      <c r="BJ5" s="149"/>
-      <c r="BK5" s="149"/>
-      <c r="BL5" s="149"/>
-      <c r="BM5" s="149"/>
-      <c r="BN5" s="149"/>
-    </row>
-    <row r="6" spans="1:143" x14ac:dyDescent="0.25">
+      <c r="BI5" s="147"/>
+      <c r="BJ5" s="147"/>
+      <c r="BK5" s="147"/>
+      <c r="BL5" s="147"/>
+      <c r="BM5" s="147"/>
+      <c r="BN5" s="147"/>
+    </row>
+    <row r="6" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A6" s="125"/>
       <c r="B6" s="123"/>
       <c r="C6" s="123"/>
@@ -4474,7 +4474,7 @@
         <v>44542</v>
       </c>
     </row>
-    <row r="7" spans="1:143" s="66" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:143" s="66" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A7" s="128" t="s">
         <v>0</v>
       </c>
@@ -4805,7 +4805,7 @@
       <c r="EL7" s="47"/>
       <c r="EM7" s="47"/>
     </row>
-    <row r="8" spans="1:143" s="42" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:143" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="134" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -4961,7 +4961,7 @@
       <c r="EL8" s="47"/>
       <c r="EM8" s="47"/>
     </row>
-    <row r="9" spans="1:143" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:143" s="44" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="108" t="str">
         <f t="shared" ref="A9:A10" si="5">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -4970,7 +4970,7 @@
         <v>136</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D9" s="101"/>
       <c r="E9" s="102">
@@ -5124,7 +5124,7 @@
       <c r="EL9" s="47"/>
       <c r="EM9" s="47"/>
     </row>
-    <row r="10" spans="1:143" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:143" s="44" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="108" t="str">
         <f t="shared" si="5"/>
         <v>1.2</v>
@@ -5133,7 +5133,7 @@
         <v>137</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D10" s="101"/>
       <c r="E10" s="102">
@@ -5287,7 +5287,7 @@
       <c r="EL10" s="47"/>
       <c r="EM10" s="47"/>
     </row>
-    <row r="11" spans="1:143" s="42" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:143" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="134" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>2</v>
@@ -5443,7 +5443,7 @@
       <c r="EL11" s="47"/>
       <c r="EM11" s="47"/>
     </row>
-    <row r="12" spans="1:143" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:143" s="44" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="108" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.1</v>
@@ -5452,7 +5452,7 @@
         <v>138</v>
       </c>
       <c r="C12" s="47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D12" s="101"/>
       <c r="E12" s="102">
@@ -5606,7 +5606,7 @@
       <c r="EL12" s="47"/>
       <c r="EM12" s="47"/>
     </row>
-    <row r="13" spans="1:143" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:143" s="44" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="108" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.2</v>
@@ -5615,7 +5615,7 @@
         <v>140</v>
       </c>
       <c r="C13" s="47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D13" s="101"/>
       <c r="E13" s="102">
@@ -5769,7 +5769,7 @@
       <c r="EL13" s="47"/>
       <c r="EM13" s="47"/>
     </row>
-    <row r="14" spans="1:143" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:143" s="44" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="108" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.3</v>
@@ -5778,7 +5778,7 @@
         <v>141</v>
       </c>
       <c r="C14" s="47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D14" s="101"/>
       <c r="E14" s="102">
@@ -5932,7 +5932,7 @@
       <c r="EL14" s="47"/>
       <c r="EM14" s="47"/>
     </row>
-    <row r="15" spans="1:143" s="42" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:143" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="134" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>3</v>
@@ -6088,7 +6088,7 @@
       <c r="EL15" s="47"/>
       <c r="EM15" s="47"/>
     </row>
-    <row r="16" spans="1:143" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:143" s="44" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="108" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.1</v>
@@ -6097,7 +6097,7 @@
         <v>144</v>
       </c>
       <c r="C16" s="47" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D16" s="101"/>
       <c r="E16" s="102">
@@ -6251,7 +6251,7 @@
       <c r="EL16" s="47"/>
       <c r="EM16" s="47"/>
     </row>
-    <row r="17" spans="1:143" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:143" s="44" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="108" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.2</v>
@@ -6260,7 +6260,7 @@
         <v>143</v>
       </c>
       <c r="C17" s="47" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D17" s="101"/>
       <c r="E17" s="102">
@@ -6414,7 +6414,7 @@
       <c r="EL17" s="47"/>
       <c r="EM17" s="47"/>
     </row>
-    <row r="18" spans="1:143" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:143" s="44" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="108" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.3</v>
@@ -6575,7 +6575,7 @@
       <c r="EL18" s="47"/>
       <c r="EM18" s="47"/>
     </row>
-    <row r="19" spans="1:143" s="42" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:143" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="134" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>4</v>
@@ -6731,7 +6731,7 @@
       <c r="EL19" s="47"/>
       <c r="EM19" s="47"/>
     </row>
-    <row r="20" spans="1:143" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:143" s="44" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="108" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.1</v>
@@ -6740,7 +6740,7 @@
         <v>145</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D20" s="101"/>
       <c r="E20" s="102">
@@ -6894,16 +6894,16 @@
       <c r="EL20" s="47"/>
       <c r="EM20" s="47"/>
     </row>
-    <row r="21" spans="1:143" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:143" s="44" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="108" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.2</v>
       </c>
       <c r="B21" s="109" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D21" s="101"/>
       <c r="E21" s="102">
@@ -7057,16 +7057,16 @@
       <c r="EL21" s="47"/>
       <c r="EM21" s="47"/>
     </row>
-    <row r="22" spans="1:143" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:143" s="44" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="108" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.3</v>
       </c>
       <c r="B22" s="109" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D22" s="101"/>
       <c r="E22" s="102">
@@ -7220,7 +7220,7 @@
       <c r="EL22" s="47"/>
       <c r="EM22" s="47"/>
     </row>
-    <row r="23" spans="1:143" s="42" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:143" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="134" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>5</v>
@@ -7376,7 +7376,7 @@
       <c r="EL23" s="47"/>
       <c r="EM23" s="47"/>
     </row>
-    <row r="24" spans="1:143" s="47" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:143" s="47" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="108" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
@@ -7385,7 +7385,7 @@
         <v>149</v>
       </c>
       <c r="C24" s="47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D24" s="101"/>
       <c r="E24" s="102">
@@ -7399,7 +7399,7 @@
         <v>7</v>
       </c>
       <c r="H24" s="105">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="I24" s="106">
         <v>7</v>
@@ -7462,7 +7462,7 @@
       <c r="BM24" s="145"/>
       <c r="BN24" s="145"/>
     </row>
-    <row r="25" spans="1:143" s="47" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:143" s="47" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="134" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>6</v>
@@ -7541,16 +7541,16 @@
       <c r="BM25" s="144"/>
       <c r="BN25" s="144"/>
     </row>
-    <row r="26" spans="1:143" s="47" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:143" s="47" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="108" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>6.1</v>
       </c>
       <c r="B26" s="109" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="C26" s="47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D26" s="101"/>
       <c r="E26" s="102">
@@ -7564,7 +7564,7 @@
         <v>7</v>
       </c>
       <c r="H26" s="105">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="I26" s="106">
         <v>7</v>
@@ -7627,7 +7627,7 @@
       <c r="BM26" s="145"/>
       <c r="BN26" s="145"/>
     </row>
-    <row r="27" spans="1:143" s="47" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:143" s="47" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="134" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>7</v>
@@ -7706,16 +7706,16 @@
       <c r="BM27" s="144"/>
       <c r="BN27" s="144"/>
     </row>
-    <row r="28" spans="1:143" s="47" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:143" s="47" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="108" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>7.1</v>
       </c>
       <c r="B28" s="109" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C28" s="47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D28" s="101"/>
       <c r="E28" s="102">
@@ -7792,13 +7792,13 @@
       <c r="BM28" s="145"/>
       <c r="BN28" s="145"/>
     </row>
-    <row r="29" spans="1:143" s="47" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:143" s="47" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="134" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>8</v>
       </c>
       <c r="B29" s="135" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C29" s="136"/>
       <c r="D29" s="137"/>
@@ -7871,16 +7871,16 @@
       <c r="BM29" s="144"/>
       <c r="BN29" s="144"/>
     </row>
-    <row r="30" spans="1:143" s="47" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:143" s="47" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="108" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>8.1</v>
       </c>
       <c r="B30" s="109" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C30" s="47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D30" s="101"/>
       <c r="E30" s="102">
@@ -7957,7 +7957,7 @@
       <c r="BM30" s="145"/>
       <c r="BN30" s="145"/>
     </row>
-    <row r="31" spans="1:143" s="47" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:143" s="47" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="108"/>
       <c r="B31" s="109"/>
       <c r="D31" s="101"/>
@@ -8025,7 +8025,7 @@
       <c r="BN31" s="1"/>
       <c r="BO31" s="1"/>
     </row>
-    <row r="32" spans="1:143" s="52" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:143" s="52" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="48" t="s">
         <v>1</v>
       </c>
@@ -8096,7 +8096,7 @@
       <c r="BN32" s="1"/>
       <c r="BO32" s="1"/>
     </row>
-    <row r="33" spans="1:67" s="47" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:67" s="47" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="53" t="s">
         <v>37</v>
       </c>
@@ -8167,7 +8167,7 @@
       <c r="BN33" s="1"/>
       <c r="BO33" s="1"/>
     </row>
-    <row r="34" spans="1:67" s="47" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:67" s="47" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="68" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -8247,7 +8247,7 @@
       <c r="BN34" s="1"/>
       <c r="BO34" s="1"/>
     </row>
-    <row r="35" spans="1:67" s="47" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:67" s="47" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="43" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -8327,7 +8327,7 @@
       <c r="BN35" s="1"/>
       <c r="BO35" s="1"/>
     </row>
-    <row r="36" spans="1:67" s="47" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:67" s="47" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="43" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.1</v>
@@ -8407,7 +8407,7 @@
       <c r="BN36" s="1"/>
       <c r="BO36" s="1"/>
     </row>
-    <row r="37" spans="1:67" s="47" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:67" s="47" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="43" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
         <v>1.1.1.1</v>
@@ -8487,7 +8487,7 @@
       <c r="BN37" s="1"/>
       <c r="BO37" s="1"/>
     </row>
-    <row r="38" spans="1:67" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:67" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="100" t="str">
         <f>HYPERLINK("https://vertex42.link/HowToCreateAGanttChart","► Watch How to Create a Gantt Chart in Excel")</f>
         <v>► Watch How to Create a Gantt Chart in Excel</v>
@@ -8559,12 +8559,21 @@
       <c r="BN38" s="1"/>
       <c r="BO38" s="1"/>
     </row>
-    <row r="39" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:67" x14ac:dyDescent="0.2">
       <c r="BO39" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -8575,15 +8584,6 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H32:H37 H8:H22">
@@ -8845,13 +8845,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>99060</xdr:colOff>
+                    <xdr:colOff>95250</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>121920</xdr:rowOff>
+                    <xdr:rowOff>123825</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>27</xdr:col>
-                    <xdr:colOff>106680</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>114300</xdr:rowOff>
                   </to>
@@ -9003,175 +9003,175 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="14" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="55.109375" style="14" customWidth="1"/>
-    <col min="4" max="7" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="5.5703125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" style="14" customWidth="1"/>
+    <col min="3" max="3" width="55.140625" style="14" customWidth="1"/>
+    <col min="4" max="7" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C4" s="20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C5" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C6" s="18"/>
     </row>
-    <row r="7" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="C7" s="21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C8" s="22" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C10" s="18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C11" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="C13" s="21" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:2" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" s="14" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="2:2" s="14" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" s="23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="2:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="2:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="2:2" s="14" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="2:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="2:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B29" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B30" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B31" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B32" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B34" s="23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="18" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="18" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" s="18" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" s="18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="2:2" s="14" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B42" s="23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="2:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B43" s="18" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="2:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B44" s="18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="2:2" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" s="14" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="2:2" ht="18" x14ac:dyDescent="0.25">
       <c r="B46" s="21" t="s">
         <v>22</v>
       </c>
@@ -9197,74 +9197,74 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="90.44140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="5.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="90.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>122</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="36"/>
     </row>
-    <row r="2" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="76" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:3" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="71" t="s">
         <v>89</v>
       </c>
       <c r="B4" s="33"/>
     </row>
-    <row r="5" spans="1:3" s="6" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="6" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="B5" s="77" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B7" s="77" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B9" s="76" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B11" s="75" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="150" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="150"/>
     </row>
-    <row r="14" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:3" s="72" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:3" s="72" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="80"/>
       <c r="B15" s="78" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="72" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="72" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="80"/>
       <c r="B16" s="79" t="s">
         <v>79</v>
@@ -9273,25 +9273,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="81"/>
       <c r="B17" s="79" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="81"/>
       <c r="B18" s="79" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="36" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="84"/>
       <c r="B19" s="79" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="72" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" s="72" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="80"/>
       <c r="B20" s="78" t="s">
         <v>80</v>
@@ -9300,153 +9300,153 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="81"/>
       <c r="B21" s="79" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="82"/>
       <c r="B22" s="83" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="82"/>
       <c r="B23" s="8"/>
     </row>
-    <row r="24" spans="1:3" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="150" t="s">
         <v>85</v>
       </c>
       <c r="B24" s="150"/>
     </row>
-    <row r="25" spans="1:3" s="6" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A25" s="82"/>
       <c r="B25" s="79" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="82"/>
       <c r="B26" s="79"/>
     </row>
-    <row r="27" spans="1:3" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="82"/>
       <c r="B27" s="99" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="82"/>
       <c r="B28" s="79" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="6" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A29" s="82"/>
       <c r="B29" s="79" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="82"/>
       <c r="B30" s="79"/>
     </row>
-    <row r="31" spans="1:3" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="82"/>
       <c r="B31" s="99" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="82"/>
       <c r="B32" s="79" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:2" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="82"/>
       <c r="B33" s="79" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="82"/>
       <c r="B34" s="8"/>
     </row>
-    <row r="35" spans="1:2" s="6" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A35" s="82"/>
       <c r="B35" s="79" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="82"/>
       <c r="B36" s="85" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:2" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="82"/>
       <c r="B37" s="8"/>
     </row>
-    <row r="38" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="150" t="s">
         <v>9</v>
       </c>
       <c r="B38" s="150"/>
     </row>
-    <row r="39" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B39" s="79" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:2" s="18" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:2" s="18" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B41" s="79" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:2" s="18" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:2" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B43" s="79" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B45" s="79" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="19"/>
     </row>
-    <row r="47" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B47" s="79" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" s="9"/>
     </row>
-    <row r="49" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="150" t="s">
         <v>7</v>
       </c>
       <c r="B49" s="150"/>
     </row>
-    <row r="50" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B50" s="79" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B51" s="9"/>
     </row>
-    <row r="52" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A52" s="86" t="s">
         <v>10</v>
       </c>
@@ -9454,7 +9454,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A53" s="86" t="s">
         <v>12</v>
       </c>
@@ -9462,7 +9462,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A54" s="86" t="s">
         <v>14</v>
       </c>
@@ -9470,19 +9470,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="28.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A55" s="75"/>
       <c r="B55" s="79" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="28.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A56" s="75"/>
       <c r="B56" s="79" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A57" s="86" t="s">
         <v>16</v>
       </c>
@@ -9490,19 +9490,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A58" s="75"/>
       <c r="B58" s="79" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A59" s="75"/>
       <c r="B59" s="79" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A60" s="86" t="s">
         <v>18</v>
       </c>
@@ -9510,13 +9510,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="28.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A61" s="75"/>
       <c r="B61" s="79" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A62" s="86" t="s">
         <v>108</v>
       </c>
@@ -9524,36 +9524,36 @@
         <v>109</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A63" s="87"/>
       <c r="B63" s="79" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="64" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B64" s="10"/>
     </row>
-    <row r="65" spans="1:2" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="150" t="s">
         <v>8</v>
       </c>
       <c r="B65" s="150"/>
     </row>
-    <row r="66" spans="1:2" s="18" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" s="18" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B66" s="79" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="67" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B67" s="11"/>
     </row>
-    <row r="68" spans="1:2" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="150" t="s">
         <v>5</v>
       </c>
       <c r="B68" s="150"/>
     </row>
-    <row r="69" spans="1:2" s="18" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="94" t="s">
         <v>6</v>
       </c>
@@ -9561,17 +9561,17 @@
         <v>112</v>
       </c>
     </row>
-    <row r="70" spans="1:2" s="6" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A70" s="88"/>
       <c r="B70" s="93" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="71" spans="1:2" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A71" s="88"/>
       <c r="B71" s="89"/>
     </row>
-    <row r="72" spans="1:2" s="18" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="94" t="s">
         <v>6</v>
       </c>
@@ -9579,17 +9579,17 @@
         <v>131</v>
       </c>
     </row>
-    <row r="73" spans="1:2" s="6" customFormat="1" ht="28.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A73" s="88"/>
       <c r="B73" s="93" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="74" spans="1:2" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A74" s="88"/>
       <c r="B74" s="89"/>
     </row>
-    <row r="75" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="94" t="s">
         <v>6</v>
       </c>
@@ -9597,17 +9597,17 @@
         <v>117</v>
       </c>
     </row>
-    <row r="76" spans="1:2" s="6" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" s="6" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A76" s="88"/>
       <c r="B76" s="77" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A77" s="87"/>
       <c r="B77" s="87"/>
     </row>
-    <row r="78" spans="1:2" s="18" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="94" t="s">
         <v>6</v>
       </c>
@@ -9615,17 +9615,17 @@
         <v>123</v>
       </c>
     </row>
-    <row r="79" spans="1:2" s="6" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A79" s="88"/>
       <c r="B79" s="77" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="80" spans="1:2" s="18" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" s="18" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A80" s="87"/>
       <c r="B80" s="87"/>
     </row>
-    <row r="81" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="94" t="s">
         <v>6</v>
       </c>
@@ -9633,29 +9633,29 @@
         <v>124</v>
       </c>
     </row>
-    <row r="82" spans="1:2" s="6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A82" s="88"/>
       <c r="B82" s="92" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="83" spans="1:2" s="6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A83" s="88"/>
       <c r="B83" s="92" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="84" spans="1:2" s="6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A84" s="88"/>
       <c r="B84" s="92" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="87"/>
       <c r="B85" s="91"/>
     </row>
-    <row r="86" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="94" t="s">
         <v>6</v>
       </c>
@@ -9663,29 +9663,29 @@
         <v>125</v>
       </c>
     </row>
-    <row r="87" spans="1:2" s="6" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" s="6" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A87" s="88"/>
       <c r="B87" s="77" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="88" spans="1:2" s="6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A88" s="88"/>
       <c r="B88" s="90" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="89" spans="1:2" s="6" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" s="6" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A89" s="88"/>
       <c r="B89" s="96" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A90" s="87"/>
       <c r="B90" s="87"/>
     </row>
-    <row r="91" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="94" t="s">
         <v>6</v>
       </c>
@@ -9693,13 +9693,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A92" s="75"/>
       <c r="B92" s="92" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="25" t="s">
         <v>53</v>
       </c>
@@ -9735,14 +9735,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="18" customWidth="1"/>
-    <col min="2" max="2" width="82.109375" style="18" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="5.5703125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="18" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>51</v>
       </c>
@@ -9750,163 +9750,163 @@
       <c r="C1" s="39"/>
       <c r="D1" s="39"/>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="36"/>
       <c r="B2" s="40"/>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="37"/>
       <c r="B3" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="38"/>
     </row>
-    <row r="4" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="32" t="s">
         <v>48</v>
       </c>
       <c r="C4" s="13"/>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="15"/>
       <c r="C5" s="13"/>
     </row>
-    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="16" t="s">
         <v>53</v>
       </c>
       <c r="C6" s="13"/>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="15"/>
       <c r="C7" s="13"/>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="15" t="s">
         <v>54</v>
       </c>
       <c r="C8" s="13"/>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="15"/>
       <c r="C9" s="13"/>
     </row>
-    <row r="10" spans="1:4" ht="46.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="15" t="s">
         <v>55</v>
       </c>
       <c r="C10" s="13"/>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="15"/>
       <c r="C11" s="13"/>
     </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="B12" s="15" t="s">
         <v>56</v>
       </c>
       <c r="C12" s="13"/>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="15"/>
       <c r="C13" s="13"/>
     </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C14" s="13"/>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="15"/>
       <c r="C15" s="13"/>
     </row>
-    <row r="16" spans="1:4" ht="30.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="30.75" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="15" t="s">
         <v>58</v>
       </c>
       <c r="C16" s="13"/>
     </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
       <c r="B17" s="15"/>
       <c r="C17" s="13"/>
     </row>
-    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="16" t="s">
         <v>59</v>
       </c>
       <c r="C18" s="13"/>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="31" t="s">
         <v>49</v>
       </c>
       <c r="C19" s="13"/>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
       <c r="B20" s="17"/>
       <c r="C20" s="13"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="13"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="13"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="13"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="13"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="13"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="13"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="13"/>

</xml_diff>